<commit_message>
analyzed the 4 pilots. discovered a problem with distance calculations in the excel file but only for practice trials. Fixed that
</commit_message>
<xml_diff>
--- a/docs/choosing_triplets.xlsx
+++ b/docs/choosing_triplets.xlsx
@@ -563,7 +563,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,16 +1864,16 @@
         <v>17</v>
       </c>
       <c r="B29" s="4">
-        <f t="shared" ref="B29:B38" si="12">F29-E29</f>
+        <f>F29-E29</f>
         <v>-40</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" ref="C29:C38" si="13">F29-G29</f>
+        <f>E29-G29</f>
+        <v>-32</v>
+      </c>
+      <c r="D29" s="5">
+        <f>F29-G29</f>
         <v>-72</v>
-      </c>
-      <c r="D29" s="5">
-        <f t="shared" ref="D29:D38" si="14">E29-G29</f>
-        <v>-32</v>
       </c>
       <c r="E29" s="4">
         <v>86</v>
@@ -1885,16 +1885,16 @@
         <v>118</v>
       </c>
       <c r="H29" s="5">
-        <f t="shared" ref="H29:H38" si="15">ABS(B29)</f>
+        <f>ABS(B29)</f>
         <v>40</v>
       </c>
       <c r="I29" s="5">
-        <f t="shared" ref="I29:I38" si="16">ABS(C29)</f>
+        <f>ABS(C29)</f>
+        <v>32</v>
+      </c>
+      <c r="J29" s="5">
+        <f>ABS(D29)</f>
         <v>72</v>
-      </c>
-      <c r="J29" s="5">
-        <f t="shared" ref="J29:J38" si="17">ABS(D29)</f>
-        <v>32</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>10</v>
@@ -1908,16 +1908,16 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="B30:B38" si="12">F30-E30</f>
         <v>-24</v>
       </c>
       <c r="C30" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="C30:C38" si="13">E30-G30</f>
+        <v>-40</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" ref="D30:D38" si="14">F30-G30</f>
         <v>-64</v>
-      </c>
-      <c r="D30" s="5">
-        <f t="shared" si="14"/>
-        <v>-40</v>
       </c>
       <c r="E30" s="4">
         <v>62</v>
@@ -1929,16 +1929,16 @@
         <v>102</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="H30:H38" si="15">ABS(B30)</f>
         <v>24</v>
       </c>
       <c r="I30" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="I30:I38" si="16">ABS(C30)</f>
+        <v>40</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" ref="J30:J38" si="17">ABS(D30)</f>
         <v>64</v>
-      </c>
-      <c r="J30" s="5">
-        <f t="shared" si="17"/>
-        <v>40</v>
       </c>
       <c r="K30" s="10" t="s">
         <v>10</v>
@@ -1957,11 +1957,11 @@
       </c>
       <c r="C31" s="4">
         <f t="shared" si="13"/>
-        <v>-80</v>
+        <v>-48</v>
       </c>
       <c r="D31" s="5">
         <f t="shared" si="14"/>
-        <v>-48</v>
+        <v>-80</v>
       </c>
       <c r="E31" s="4">
         <v>62</v>
@@ -1978,11 +1978,11 @@
       </c>
       <c r="I31" s="5">
         <f t="shared" si="16"/>
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="J31" s="5">
         <f t="shared" si="17"/>
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="K31" s="10" t="s">
         <v>10</v>
@@ -2001,11 +2001,11 @@
       </c>
       <c r="C32" s="4">
         <f t="shared" si="13"/>
-        <v>-16</v>
+        <v>-8</v>
       </c>
       <c r="D32" s="5">
         <f t="shared" si="14"/>
-        <v>-8</v>
+        <v>-16</v>
       </c>
       <c r="E32" s="4">
         <v>38</v>
@@ -2022,11 +2022,11 @@
       </c>
       <c r="I32" s="5">
         <f t="shared" si="16"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J32" s="5">
         <f t="shared" si="17"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K32" s="10" t="s">
         <v>10</v>
@@ -2045,11 +2045,11 @@
       </c>
       <c r="C33" s="4">
         <f t="shared" si="13"/>
-        <v>-72</v>
+        <v>-64</v>
       </c>
       <c r="D33" s="5">
         <f t="shared" si="14"/>
-        <v>-64</v>
+        <v>-72</v>
       </c>
       <c r="E33" s="4">
         <v>46</v>
@@ -2066,11 +2066,11 @@
       </c>
       <c r="I33" s="5">
         <f t="shared" si="16"/>
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J33" s="5">
         <f t="shared" si="17"/>
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="K33" s="10" t="s">
         <v>10</v>
@@ -2089,11 +2089,11 @@
       </c>
       <c r="C34" s="4">
         <f t="shared" si="13"/>
-        <v>-16</v>
+        <v>-8</v>
       </c>
       <c r="D34" s="5">
         <f t="shared" si="14"/>
-        <v>-8</v>
+        <v>-16</v>
       </c>
       <c r="E34" s="4">
         <v>110</v>
@@ -2110,11 +2110,11 @@
       </c>
       <c r="I34" s="5">
         <f t="shared" si="16"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J34" s="5">
         <f t="shared" si="17"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K34" s="10" t="s">
         <v>10</v>
@@ -2133,11 +2133,11 @@
       </c>
       <c r="C35" s="4">
         <f t="shared" si="13"/>
-        <v>-24</v>
+        <v>-16</v>
       </c>
       <c r="D35" s="5">
         <f t="shared" si="14"/>
-        <v>-16</v>
+        <v>-24</v>
       </c>
       <c r="E35" s="4">
         <v>46</v>
@@ -2154,11 +2154,11 @@
       </c>
       <c r="I35" s="5">
         <f t="shared" si="16"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J35" s="5">
         <f t="shared" si="17"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="K35" s="10" t="s">
         <v>10</v>
@@ -2177,11 +2177,11 @@
       </c>
       <c r="C36" s="4">
         <f t="shared" si="13"/>
-        <v>-80</v>
+        <v>-8</v>
       </c>
       <c r="D36" s="5">
         <f t="shared" si="14"/>
-        <v>-8</v>
+        <v>-80</v>
       </c>
       <c r="E36" s="4">
         <v>110</v>
@@ -2198,11 +2198,11 @@
       </c>
       <c r="I36" s="5">
         <f t="shared" si="16"/>
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="J36" s="5">
         <f t="shared" si="17"/>
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="K36" s="10" t="s">
         <v>10</v>
@@ -2221,11 +2221,11 @@
       </c>
       <c r="C37" s="4">
         <f t="shared" si="13"/>
-        <v>-80</v>
+        <v>-64</v>
       </c>
       <c r="D37" s="5">
         <f t="shared" si="14"/>
-        <v>-64</v>
+        <v>-80</v>
       </c>
       <c r="E37" s="4">
         <v>46</v>
@@ -2242,11 +2242,11 @@
       </c>
       <c r="I37" s="5">
         <f t="shared" si="16"/>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="J37" s="5">
         <f t="shared" si="17"/>
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="K37" s="10" t="s">
         <v>10</v>
@@ -2265,11 +2265,11 @@
       </c>
       <c r="C38" s="4">
         <f t="shared" si="13"/>
-        <v>-88</v>
+        <v>-48</v>
       </c>
       <c r="D38" s="5">
         <f t="shared" si="14"/>
-        <v>-48</v>
+        <v>-88</v>
       </c>
       <c r="E38" s="4">
         <v>70</v>
@@ -2286,11 +2286,11 @@
       </c>
       <c r="I38" s="5">
         <f t="shared" si="16"/>
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="J38" s="5">
         <f t="shared" si="17"/>
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="K38" s="10" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
deleted some files from the previous pilot paradigm
</commit_message>
<xml_diff>
--- a/docs/choosing_triplets.xlsx
+++ b/docs/choosing_triplets.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb08\GitHub\density_2_analysis\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\density_2_analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8DC42B-5F75-4657-9022-CF7C44350935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="12180" windowWidth="23250" windowHeight="12570" tabRatio="358"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="358" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$L$94</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="16">
   <si>
     <t>simulation name</t>
   </si>
@@ -86,17 +88,11 @@
   <si>
     <t>regular</t>
   </si>
-  <si>
-    <t>practice</t>
-  </si>
-  <si>
-    <t>balancing</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -558,12 +554,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,15 +676,15 @@
         <v>-16</v>
       </c>
       <c r="E3" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F3" s="13">
         <f>E3-Sheet2!$B$1</f>
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G3" s="13">
         <f>E3+Sheet2!$B$1</f>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ref="H3:H28" si="3">ABS(B3)</f>
@@ -726,15 +722,15 @@
         <v>-16</v>
       </c>
       <c r="E4" s="5">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F4" s="13">
         <f>E4-Sheet2!$B$1</f>
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G4" s="13">
         <f>E4+Sheet2!$B$1</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="3"/>
@@ -818,15 +814,15 @@
         <v>-32</v>
       </c>
       <c r="E6" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F6" s="13">
         <f>E6-Sheet2!$B$1*2</f>
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G6" s="13">
         <f>E6+Sheet2!$B$1*2</f>
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="3"/>
@@ -864,15 +860,16 @@
         <v>-32</v>
       </c>
       <c r="E7" s="5">
-        <v>102</v>
+        <f>102-8</f>
+        <v>94</v>
       </c>
       <c r="F7" s="13">
         <f>E7-Sheet2!$B$1*2</f>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G7" s="13">
         <f>E7+Sheet2!$B$1*2</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="3"/>
@@ -956,15 +953,15 @@
         <v>-48</v>
       </c>
       <c r="E9" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F9" s="13">
         <f>E9-Sheet2!$B$1*3</f>
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G9" s="13">
         <f>E9+Sheet2!$B$1*3</f>
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="3"/>
@@ -1002,15 +999,15 @@
         <v>-48</v>
       </c>
       <c r="E10" s="5">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F10" s="13">
         <f>E10-Sheet2!$B$1*3</f>
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G10" s="13">
         <f>E10+Sheet2!$B$1*3</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="3"/>
@@ -1094,15 +1091,15 @@
         <v>-24</v>
       </c>
       <c r="E12" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F12" s="13">
         <f>E12-Sheet2!$B$1*1</f>
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G12" s="13">
         <f>E12+Sheet2!$B$1*2</f>
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="3"/>
@@ -1140,15 +1137,15 @@
         <v>-24</v>
       </c>
       <c r="E13" s="5">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F13" s="13">
         <f>E13-Sheet2!$B$1*1</f>
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G13" s="13">
         <f>E13+Sheet2!$B$1*2</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="3"/>
@@ -1232,15 +1229,15 @@
         <v>-24</v>
       </c>
       <c r="E15" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F15" s="13">
         <f>E15-Sheet2!$B$1*2</f>
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G15" s="13">
         <f>E15+Sheet2!$B$1*1</f>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="3"/>
@@ -1278,15 +1275,15 @@
         <v>-24</v>
       </c>
       <c r="E16" s="5">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F16" s="13">
         <f>E16-Sheet2!$B$1*2</f>
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G16" s="13">
         <f>E16+Sheet2!$B$1*1</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="3"/>
@@ -1370,15 +1367,15 @@
         <v>-40</v>
       </c>
       <c r="E18" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F18" s="13">
         <f>E18-Sheet2!$B$1*2</f>
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G18" s="13">
         <f>E18+Sheet2!$B$1*3</f>
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="3"/>
@@ -1416,15 +1413,15 @@
         <v>-40</v>
       </c>
       <c r="E19" s="5">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F19" s="13">
         <f>E19-Sheet2!$B$1*2</f>
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G19" s="13">
         <f>E19+Sheet2!$B$1*3</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="3"/>
@@ -1508,15 +1505,15 @@
         <v>-40</v>
       </c>
       <c r="E21" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F21" s="13">
         <f>E21-Sheet2!$B$1*3</f>
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G21" s="13">
         <f>E21+Sheet2!$B$1*2</f>
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="3"/>
@@ -1554,15 +1551,15 @@
         <v>-40</v>
       </c>
       <c r="E22" s="5">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F22" s="13">
         <f>E22-Sheet2!$B$1*3</f>
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G22" s="13">
         <f>E22+Sheet2!$B$1*2</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" si="3"/>
@@ -1646,15 +1643,15 @@
         <v>-32</v>
       </c>
       <c r="E24" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F24" s="13">
         <f>E24-Sheet2!$B$1*1</f>
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G24" s="13">
         <f>E24+Sheet2!$B$1*3</f>
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H24" s="5">
         <f t="shared" si="3"/>
@@ -1692,15 +1689,15 @@
         <v>-32</v>
       </c>
       <c r="E25" s="5">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F25" s="13">
         <f>E25-Sheet2!$B$1*1</f>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G25" s="13">
         <f>E25+Sheet2!$B$1*3</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H25" s="5">
         <f t="shared" si="3"/>
@@ -1784,15 +1781,15 @@
         <v>-32</v>
       </c>
       <c r="E27" s="5">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F27" s="13">
         <f>E27-Sheet2!$B$1*3</f>
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G27" s="13">
         <f>E27+Sheet2!$B$1*1</f>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H27" s="5">
         <f t="shared" si="3"/>
@@ -1830,15 +1827,15 @@
         <v>-32</v>
       </c>
       <c r="E28" s="5">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F28" s="13">
         <f>E28-Sheet2!$B$1*3</f>
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G28" s="13">
         <f>E28+Sheet2!$B$1*1</f>
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H28" s="5">
         <f t="shared" si="3"/>
@@ -1860,444 +1857,144 @@
       </c>
     </row>
     <row r="29" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="4">
-        <f>F29-E29</f>
-        <v>-40</v>
-      </c>
-      <c r="C29" s="4">
-        <f>E29-G29</f>
-        <v>-32</v>
-      </c>
-      <c r="D29" s="5">
-        <f>F29-G29</f>
-        <v>-72</v>
-      </c>
-      <c r="E29" s="4">
-        <v>86</v>
-      </c>
-      <c r="F29" s="4">
-        <v>46</v>
-      </c>
-      <c r="G29" s="4">
-        <v>118</v>
-      </c>
-      <c r="H29" s="5">
-        <f>ABS(B29)</f>
-        <v>40</v>
-      </c>
-      <c r="I29" s="5">
-        <f>ABS(C29)</f>
-        <v>32</v>
-      </c>
-      <c r="J29" s="5">
-        <f>ABS(D29)</f>
-        <v>72</v>
-      </c>
-      <c r="K29" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="4">
-        <f t="shared" ref="B30:B38" si="12">F30-E30</f>
-        <v>-24</v>
-      </c>
-      <c r="C30" s="4">
-        <f t="shared" ref="C30:C38" si="13">E30-G30</f>
-        <v>-40</v>
-      </c>
-      <c r="D30" s="5">
-        <f t="shared" ref="D30:D38" si="14">F30-G30</f>
-        <v>-64</v>
-      </c>
-      <c r="E30" s="4">
-        <v>62</v>
-      </c>
-      <c r="F30" s="4">
-        <v>38</v>
-      </c>
-      <c r="G30" s="4">
-        <v>102</v>
-      </c>
-      <c r="H30" s="5">
-        <f t="shared" ref="H30:H38" si="15">ABS(B30)</f>
-        <v>24</v>
-      </c>
-      <c r="I30" s="5">
-        <f t="shared" ref="I30:I38" si="16">ABS(C30)</f>
-        <v>40</v>
-      </c>
-      <c r="J30" s="5">
-        <f t="shared" ref="J30:J38" si="17">ABS(D30)</f>
-        <v>64</v>
-      </c>
-      <c r="K30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="4">
-        <f t="shared" si="12"/>
-        <v>-32</v>
-      </c>
-      <c r="C31" s="4">
-        <f t="shared" si="13"/>
-        <v>-48</v>
-      </c>
-      <c r="D31" s="5">
-        <f t="shared" si="14"/>
-        <v>-80</v>
-      </c>
-      <c r="E31" s="4">
-        <v>62</v>
-      </c>
-      <c r="F31" s="4">
-        <v>30</v>
-      </c>
-      <c r="G31" s="4">
-        <v>110</v>
-      </c>
-      <c r="H31" s="5">
-        <f t="shared" si="15"/>
-        <v>32</v>
-      </c>
-      <c r="I31" s="5">
-        <f t="shared" si="16"/>
-        <v>48</v>
-      </c>
-      <c r="J31" s="5">
-        <f t="shared" si="17"/>
-        <v>80</v>
-      </c>
-      <c r="K31" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="4">
-        <f t="shared" si="12"/>
-        <v>-8</v>
-      </c>
-      <c r="C32" s="4">
-        <f t="shared" si="13"/>
-        <v>-8</v>
-      </c>
-      <c r="D32" s="5">
-        <f t="shared" si="14"/>
-        <v>-16</v>
-      </c>
-      <c r="E32" s="4">
-        <v>38</v>
-      </c>
-      <c r="F32" s="4">
-        <v>30</v>
-      </c>
-      <c r="G32" s="4">
-        <v>46</v>
-      </c>
-      <c r="H32" s="5">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="I32" s="5">
-        <f t="shared" si="16"/>
-        <v>8</v>
-      </c>
-      <c r="J32" s="5">
-        <f t="shared" si="17"/>
-        <v>16</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="4">
-        <f t="shared" si="12"/>
-        <v>-8</v>
-      </c>
-      <c r="C33" s="4">
-        <f t="shared" si="13"/>
-        <v>-64</v>
-      </c>
-      <c r="D33" s="5">
-        <f t="shared" si="14"/>
-        <v>-72</v>
-      </c>
-      <c r="E33" s="4">
-        <v>46</v>
-      </c>
-      <c r="F33" s="4">
-        <v>38</v>
-      </c>
-      <c r="G33" s="4">
-        <v>110</v>
-      </c>
-      <c r="H33" s="5">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="I33" s="5">
-        <f t="shared" si="16"/>
-        <v>64</v>
-      </c>
-      <c r="J33" s="5">
-        <f t="shared" si="17"/>
-        <v>72</v>
-      </c>
-      <c r="K33" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" s="4">
-        <f t="shared" si="12"/>
-        <v>-8</v>
-      </c>
-      <c r="C34" s="4">
-        <f t="shared" si="13"/>
-        <v>-8</v>
-      </c>
-      <c r="D34" s="5">
-        <f t="shared" si="14"/>
-        <v>-16</v>
-      </c>
-      <c r="E34" s="4">
-        <v>110</v>
-      </c>
-      <c r="F34" s="4">
-        <v>102</v>
-      </c>
-      <c r="G34" s="4">
-        <v>118</v>
-      </c>
-      <c r="H34" s="5">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="I34" s="5">
-        <f t="shared" si="16"/>
-        <v>8</v>
-      </c>
-      <c r="J34" s="5">
-        <f t="shared" si="17"/>
-        <v>16</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="4">
-        <f t="shared" si="12"/>
-        <v>-8</v>
-      </c>
-      <c r="C35" s="4">
-        <f t="shared" si="13"/>
-        <v>-16</v>
-      </c>
-      <c r="D35" s="5">
-        <f t="shared" si="14"/>
-        <v>-24</v>
-      </c>
-      <c r="E35" s="4">
-        <v>46</v>
-      </c>
-      <c r="F35" s="4">
-        <v>38</v>
-      </c>
-      <c r="G35" s="4">
-        <v>62</v>
-      </c>
-      <c r="H35" s="5">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="I35" s="5">
-        <f t="shared" si="16"/>
-        <v>16</v>
-      </c>
-      <c r="J35" s="5">
-        <f t="shared" si="17"/>
-        <v>24</v>
-      </c>
-      <c r="K35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A35" s="3"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="4">
-        <f t="shared" si="12"/>
-        <v>-72</v>
-      </c>
-      <c r="C36" s="4">
-        <f t="shared" si="13"/>
-        <v>-8</v>
-      </c>
-      <c r="D36" s="5">
-        <f t="shared" si="14"/>
-        <v>-80</v>
-      </c>
-      <c r="E36" s="4">
-        <v>110</v>
-      </c>
-      <c r="F36" s="4">
-        <v>38</v>
-      </c>
-      <c r="G36" s="4">
-        <v>118</v>
-      </c>
-      <c r="H36" s="5">
-        <f t="shared" si="15"/>
-        <v>72</v>
-      </c>
-      <c r="I36" s="5">
-        <f t="shared" si="16"/>
-        <v>8</v>
-      </c>
-      <c r="J36" s="5">
-        <f t="shared" si="17"/>
-        <v>80</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="4">
-        <f t="shared" si="12"/>
-        <v>-16</v>
-      </c>
-      <c r="C37" s="4">
-        <f t="shared" si="13"/>
-        <v>-64</v>
-      </c>
-      <c r="D37" s="5">
-        <f t="shared" si="14"/>
-        <v>-80</v>
-      </c>
-      <c r="E37" s="4">
-        <v>46</v>
-      </c>
-      <c r="F37" s="4">
-        <v>30</v>
-      </c>
-      <c r="G37" s="4">
-        <v>110</v>
-      </c>
-      <c r="H37" s="5">
-        <f t="shared" si="15"/>
-        <v>16</v>
-      </c>
-      <c r="I37" s="5">
-        <f t="shared" si="16"/>
-        <v>64</v>
-      </c>
-      <c r="J37" s="5">
-        <f t="shared" si="17"/>
-        <v>80</v>
-      </c>
-      <c r="K37" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A37" s="3"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="4">
-        <f t="shared" si="12"/>
-        <v>-40</v>
-      </c>
-      <c r="C38" s="4">
-        <f t="shared" si="13"/>
-        <v>-48</v>
-      </c>
-      <c r="D38" s="5">
-        <f t="shared" si="14"/>
-        <v>-88</v>
-      </c>
-      <c r="E38" s="4">
-        <v>70</v>
-      </c>
-      <c r="F38" s="4">
-        <v>30</v>
-      </c>
-      <c r="G38" s="4">
-        <v>118</v>
-      </c>
-      <c r="H38" s="5">
-        <f t="shared" si="15"/>
-        <v>40</v>
-      </c>
-      <c r="I38" s="5">
-        <f t="shared" si="16"/>
-        <v>48</v>
-      </c>
-      <c r="J38" s="5">
-        <f t="shared" si="17"/>
-        <v>88</v>
-      </c>
-      <c r="K38" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
@@ -3077,14 +2774,14 @@
       <c r="L94" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L94"/>
+  <autoFilter ref="A1:L94" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
settled on the new balancing triplets. Decided that 70 is included in exposure ones
</commit_message>
<xml_diff>
--- a/docs/choosing_triplets.xlsx
+++ b/docs/choosing_triplets.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levan\GitHub\density_2_analysis\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lb08\GitHub\density_2_analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8DC42B-5F75-4657-9022-CF7C44350935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="358" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="10380" tabRatio="358"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$L$94</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="18">
   <si>
     <t>simulation name</t>
   </si>
@@ -88,11 +87,17 @@
   <si>
     <t>regular</t>
   </si>
+  <si>
+    <t>balancing</t>
+  </si>
+  <si>
+    <t>practice</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -554,12 +559,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,144 +1862,444 @@
       </c>
     </row>
     <row r="29" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="5"/>
+      <c r="A29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" ref="B29:B38" si="12">E29-F29</f>
+        <v>8</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" ref="C29:C38" si="13">E29-G29</f>
+        <v>-72</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" ref="D29:D38" si="14">F29-G29</f>
+        <v>-80</v>
+      </c>
+      <c r="E29" s="4">
+        <v>38</v>
+      </c>
+      <c r="F29" s="4">
+        <v>30</v>
+      </c>
+      <c r="G29" s="4">
+        <v>110</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" ref="H29:H38" si="15">ABS(B29)</f>
+        <v>8</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" ref="I29:I38" si="16">ABS(C29)</f>
+        <v>72</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" ref="J29:J38" si="17">ABS(D29)</f>
+        <v>80</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="30" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="5"/>
+      <c r="A30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="13"/>
+        <v>-64</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="14"/>
+        <v>-72</v>
+      </c>
+      <c r="E30" s="4">
+        <v>38</v>
+      </c>
+      <c r="F30" s="4">
+        <v>30</v>
+      </c>
+      <c r="G30" s="4">
+        <v>102</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" si="16"/>
+        <v>64</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="17"/>
+        <v>72</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="5"/>
+      <c r="A31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="12"/>
+        <v>56</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="13"/>
+        <v>-16</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="14"/>
+        <v>-72</v>
+      </c>
+      <c r="E31" s="4">
+        <v>94</v>
+      </c>
+      <c r="F31" s="4">
+        <v>38</v>
+      </c>
+      <c r="G31" s="4">
+        <v>110</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="15"/>
+        <v>56</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" si="16"/>
+        <v>16</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="17"/>
+        <v>72</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="32" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="5"/>
+      <c r="A32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="13"/>
+        <v>-16</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="14"/>
+        <v>-24</v>
+      </c>
+      <c r="E32" s="4">
+        <v>38</v>
+      </c>
+      <c r="F32" s="4">
+        <v>30</v>
+      </c>
+      <c r="G32" s="4">
+        <v>54</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="I32" s="5">
+        <f t="shared" si="16"/>
+        <v>16</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="17"/>
+        <v>24</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="33" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="5"/>
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="12"/>
+        <v>16</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="13"/>
+        <v>-8</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="14"/>
+        <v>-24</v>
+      </c>
+      <c r="E33" s="4">
+        <v>102</v>
+      </c>
+      <c r="F33" s="4">
+        <v>86</v>
+      </c>
+      <c r="G33" s="4">
+        <v>110</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="15"/>
+        <v>16</v>
+      </c>
+      <c r="I33" s="5">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="17"/>
+        <v>24</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="5"/>
+      <c r="A34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" si="12"/>
+        <v>32</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="13"/>
+        <v>-40</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="14"/>
+        <v>-72</v>
+      </c>
+      <c r="E34" s="4">
+        <v>62</v>
+      </c>
+      <c r="F34" s="4">
+        <v>30</v>
+      </c>
+      <c r="G34" s="4">
+        <v>102</v>
+      </c>
+      <c r="H34" s="5">
+        <f t="shared" si="15"/>
+        <v>32</v>
+      </c>
+      <c r="I34" s="5">
+        <f t="shared" si="16"/>
+        <v>40</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="17"/>
+        <v>72</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="35" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="5"/>
+      <c r="A35" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" si="12"/>
+        <v>32</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="13"/>
+        <v>-32</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="14"/>
+        <v>-64</v>
+      </c>
+      <c r="E35" s="4">
+        <v>78</v>
+      </c>
+      <c r="F35" s="4">
+        <v>46</v>
+      </c>
+      <c r="G35" s="4">
+        <v>110</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" si="15"/>
+        <v>32</v>
+      </c>
+      <c r="I35" s="5">
+        <f t="shared" si="16"/>
+        <v>32</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="17"/>
+        <v>64</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="36" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="5"/>
+      <c r="A36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="13"/>
+        <v>-8</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" si="14"/>
+        <v>-16</v>
+      </c>
+      <c r="E36" s="4">
+        <v>102</v>
+      </c>
+      <c r="F36" s="4">
+        <v>94</v>
+      </c>
+      <c r="G36" s="4">
+        <v>110</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="I36" s="5">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" si="17"/>
+        <v>16</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="37" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="5"/>
+      <c r="A37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="4">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="13"/>
+        <v>-64</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="14"/>
+        <v>-72</v>
+      </c>
+      <c r="E37" s="4">
+        <v>38</v>
+      </c>
+      <c r="F37" s="4">
+        <v>30</v>
+      </c>
+      <c r="G37" s="4">
+        <v>102</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="I37" s="5">
+        <f t="shared" si="16"/>
+        <v>64</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="17"/>
+        <v>72</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="38" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="5"/>
+      <c r="A38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="4">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="13"/>
+        <v>-56</v>
+      </c>
+      <c r="D38" s="5">
+        <f t="shared" si="14"/>
+        <v>-64</v>
+      </c>
+      <c r="E38" s="4">
+        <v>46</v>
+      </c>
+      <c r="F38" s="4">
+        <v>38</v>
+      </c>
+      <c r="G38" s="4">
+        <v>102</v>
+      </c>
+      <c r="H38" s="5">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="I38" s="5">
+        <f t="shared" si="16"/>
+        <v>56</v>
+      </c>
+      <c r="J38" s="5">
+        <f t="shared" si="17"/>
+        <v>64</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="39" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
@@ -2774,14 +3079,14 @@
       <c r="L94" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L94" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L94"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>